<commit_message>
added chapter with structured patterns to patterns list
</commit_message>
<xml_diff>
--- a/Patterns.xlsx
+++ b/Patterns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="123">
   <si>
     <t>Одиночка</t>
   </si>
@@ -236,12 +236,244 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Адаптер</t>
+  </si>
+  <si>
+    <t>Обёртка, Adapter</t>
+  </si>
+  <si>
+    <t> Отделяет и скрывает от клиента подробности преобразования различных интерфейсов.</t>
+  </si>
+  <si>
+    <t>Усложняет код программы из-за введения дополнительных классов.</t>
+  </si>
+  <si>
+    <t> Когда вы хотите использовать сторонний класс, но его интерфейс не соответствует остальному коду приложения.</t>
+  </si>
+  <si>
+    <t> Когда вам нужно использовать несколько существующих подклассов, но в них не хватает какой-то общей функциональности, причём расширить суперкласс вы не можете.</t>
+  </si>
+  <si>
+    <t> разделяет один или несколько классов на две отдельные иерархии — абстракцию и реализацию, позволяя изменять их независимо друг от друга.</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Когда вы хотите разделить монолитный класс, который содержит несколько различных реализаций какой-то функциональности (например, если класс может работать с разными системами баз данных).</t>
+  </si>
+  <si>
+    <t>Когда класс нужно расширять в двух независимых плоскостях.</t>
+  </si>
+  <si>
+    <t> Когда вы хотите, чтобы реализацию можно было бы изменять во время выполнения программы.</t>
+  </si>
+  <si>
+    <t>Позволяет строить платформо-независимые программы.</t>
+  </si>
+  <si>
+    <t> Скрывает лишние или опасные детали реализации от клиентского кода.</t>
+  </si>
+  <si>
+    <t> Усложняет код программы из-за введения дополнительных классов</t>
+  </si>
+  <si>
+    <t>Мост </t>
+  </si>
+  <si>
+    <t>Компоновщик</t>
+  </si>
+  <si>
+    <t>Дерево, Composite</t>
+  </si>
+  <si>
+    <t> Когда вам нужно представить древовидную структуру объектов.</t>
+  </si>
+  <si>
+    <t> Когда клиенты должны единообразно трактовать простые и составные объекты</t>
+  </si>
+  <si>
+    <t> Упрощает архитектуру клиента при работе со сложным деревом компонентов.</t>
+  </si>
+  <si>
+    <t> Облегчает добавление новых видов компонентов.</t>
+  </si>
+  <si>
+    <t> Создаёт слишком общий дизайн классов.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> позволяет сгруппировать множество объектов в древовидную структуру, а затем работать с ней так, как будто это единичный объект.</t>
+  </si>
+  <si>
+    <t>позволяет объектам с несовместимыми интерфейсами работать вместе.</t>
+  </si>
+  <si>
+    <t>Декоратор</t>
+  </si>
+  <si>
+    <t>Обёртка, Decorator</t>
+  </si>
+  <si>
+    <t> динамически добавлять объектам новую функциональность, оборачивая их в полезные «обёртки». Простыми словами как наследование заменить композицией</t>
+  </si>
+  <si>
+    <t> Когда вам нужно добавлять обязанности объектам на лету, незаметно для кода, который их использует.</t>
+  </si>
+  <si>
+    <t> Когда нельзя расширить обязанности объекта с помощью наследования.</t>
+  </si>
+  <si>
+    <t>Большая гибкость, чем у наследования.</t>
+  </si>
+  <si>
+    <t>Позволяет добавлять обязанности на лету.</t>
+  </si>
+  <si>
+    <t>Можно добавлять несколько новых обязанностей сразу.</t>
+  </si>
+  <si>
+    <t>Позволяет иметь несколько мелких объектов вместо одного объекта на все случаи жизни.</t>
+  </si>
+  <si>
+    <t>Трудно конфигурировать многократно обёрнутые объекты.</t>
+  </si>
+  <si>
+    <t>Обилие крошечных классов.</t>
+  </si>
+  <si>
+    <t>Фасад</t>
+  </si>
+  <si>
+    <t> предоставляет простой интерфейс к сложной системе классов, библиотеке или фреймворку</t>
+  </si>
+  <si>
+    <t>Когда вам нужно представить простой или урезанный интерфейс к сложной подсистеме.</t>
+  </si>
+  <si>
+    <t> Когда вы хотите разложить подсистему на отдельные слои.</t>
+  </si>
+  <si>
+    <t>Facade</t>
+  </si>
+  <si>
+    <t> Изолирует клиентов от компонентов сложной подсистемы.</t>
+  </si>
+  <si>
+    <t>Фасад рискует стать божественным объектом, привязанным ко всем классам программы.</t>
+  </si>
+  <si>
+    <t>Легковес</t>
+  </si>
+  <si>
+    <t>Приспособленец, Кэш, Flyweight</t>
+  </si>
+  <si>
+    <t> позволяет вместить бóльшее количество объектов в отведённую оперативную память. Легковес экономит память, разделяя общее состояние объектов между собой, вместо хранения одинаковых данных в каждом объекте.</t>
+  </si>
+  <si>
+    <t> Когда не хватает оперативной памяти для поддержки всех нужных объектов</t>
+  </si>
+  <si>
+    <t>в приложении используется большое число объектов;</t>
+  </si>
+  <si>
+    <t>из-за этого высоки расходы оперативной памяти;</t>
+  </si>
+  <si>
+    <t>большую часть состояния объектов можно вынести за пределы их классов;</t>
+  </si>
+  <si>
+    <t>большие группы объектов можно заменить относительно небольшим количеством разделяемых объектов, поскольку внешнее состояние вынесено.</t>
+  </si>
+  <si>
+    <t> Экономит оперативную память</t>
+  </si>
+  <si>
+    <t> Расходует процессорное время на поиск/вычисление контекста.</t>
+  </si>
+  <si>
+    <t>Заместитель</t>
+  </si>
+  <si>
+    <t>Proxy</t>
+  </si>
+  <si>
+    <t>Ленивая инициализация (виртуальный прокси). Когда у вас есть тяжёлый объект, грузящий данные из файловой системы или базы данных.</t>
+  </si>
+  <si>
+    <t> Защита доступа (защищающий прокси). Когда в программе есть разные типы пользователей, и вам хочется защищать объект от неавторизованного доступа. </t>
+  </si>
+  <si>
+    <t>Локальный запуск сервиса (удалённый прокси). Когда настоящий сервисный объект находится на удалённом сервере.</t>
+  </si>
+  <si>
+    <t> Логирование запросов (логирующий прокси). Когда требуется хранить историю обращений к сервисному объекту.</t>
+  </si>
+  <si>
+    <t>Кеширование объектов («умная» ссылка). Когда нужно кешировать результаты запросов клиентов и управлять их жизненным циклом</t>
+  </si>
+  <si>
+    <t> Позволяет контролировать сервисный объект незаметно для клиента.</t>
+  </si>
+  <si>
+    <t> Может работать, даже если сервисный объект ещё не создан.</t>
+  </si>
+  <si>
+    <t> Может контролировать жизненный цикл служебного объекта.</t>
+  </si>
+  <si>
+    <t> Увеличивает время отклика от сервиса.</t>
+  </si>
+  <si>
+    <r>
+      <t> позволяет подставлять вместо реальных объектов специальные объекты-заменители. Эти объекты перехватывают вызовы к оригинальному объекту, позволяя сделать что-то </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>до</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> или </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>после</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>передачи вызова оригиналу</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +518,47 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,8 +571,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEA694"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -402,6 +679,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -410,7 +829,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,112 +887,285 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -583,6 +1175,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFEA694"/>
       <color rgb="FF3FFF96"/>
       <color rgb="FFA7FBDF"/>
     </mruColors>
@@ -875,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -890,46 +1483,47 @@
     <col min="5" max="5" width="52.7109375" style="14" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" style="14" customWidth="1"/>
     <col min="7" max="7" width="47.7109375" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="14"/>
+    <col min="8" max="8" width="45.7109375" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="13.5" thickBot="1">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="39.75" customHeight="1">
-      <c r="A3" s="58">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="50" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -937,10 +1531,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5">
-      <c r="A4" s="58"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="40"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
@@ -952,10 +1546,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5">
-      <c r="A5" s="58"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="40"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
         <v>5</v>
@@ -965,27 +1559,27 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A6" s="58"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="51">
-      <c r="A7" s="58">
+      <c r="A7" s="32">
         <v>2</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="39" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -994,15 +1588,15 @@
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A8" s="58"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="47"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1012,10 +1606,10 @@
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A9" s="58"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="47"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="57"/>
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1025,10 +1619,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A10" s="58"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="49"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="9"/>
       <c r="F10" s="11" t="s">
         <v>28</v>
@@ -1036,22 +1630,22 @@
       <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7" ht="38.25">
-      <c r="A11" s="58">
+      <c r="A11" s="32">
         <v>3</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1059,14 +1653,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="38.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="29"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -1074,49 +1668,49 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5">
-      <c r="A13" s="58"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="29"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" ht="25.5">
-      <c r="A14" s="58"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="29"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="24" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A15" s="58"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="52"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="25.5">
-      <c r="A16" s="58">
+      <c r="A16" s="32">
         <v>4</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="47" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1130,10 +1724,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="38.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="48"/>
       <c r="E17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1145,10 +1739,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A18" s="58"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="55"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="18" t="s">
         <v>35</v>
       </c>
@@ -1158,16 +1752,16 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="25.5">
-      <c r="A19" s="58">
+      <c r="A19" s="32">
         <v>5</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="39" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1181,10 +1775,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="51">
-      <c r="A20" s="58"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="56"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="5" t="s">
         <v>46</v>
       </c>
@@ -1194,10 +1788,10 @@
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="58"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="56"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="5"/>
       <c r="F21" s="21" t="s">
         <v>49</v>
@@ -1205,18 +1799,443 @@
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A22" s="58"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="57"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="10"/>
       <c r="F22" s="22" t="s">
         <v>50</v>
       </c>
       <c r="G22" s="16"/>
     </row>
+    <row r="23" spans="1:7" ht="13.5" thickBot="1"/>
+    <row r="24" spans="1:7" ht="38.25">
+      <c r="B24" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="83" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="85" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="51.75" thickBot="1">
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="51">
+      <c r="B26" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="64"/>
+    </row>
+    <row r="27" spans="1:7" ht="25.5">
+      <c r="B27" s="90"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="65"/>
+    </row>
+    <row r="28" spans="1:7" ht="26.25" thickBot="1">
+      <c r="B28" s="93"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:7" ht="25.5">
+      <c r="B29" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="96" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="26.25" thickBot="1">
+      <c r="B30" s="97"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="99" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="99" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="66"/>
+    </row>
+    <row r="31" spans="1:7" ht="25.5">
+      <c r="B31" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="25.5">
+      <c r="B32" s="100"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="25.5">
+      <c r="B33" s="100"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="67"/>
+    </row>
+    <row r="34" spans="2:7" ht="26.25" thickBot="1">
+      <c r="B34" s="101"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="68"/>
+    </row>
+    <row r="35" spans="2:7" ht="25.5">
+      <c r="B35" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="103" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="26.25" thickBot="1">
+      <c r="B36" s="97"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="60"/>
+      <c r="G36" s="68"/>
+    </row>
+    <row r="37" spans="2:7" ht="25.5">
+      <c r="B37" s="107" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="108" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="109" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="25.5">
+      <c r="B38" s="110"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="111" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="59"/>
+      <c r="G38" s="67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="110"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="111" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="59"/>
+      <c r="G39" s="67"/>
+    </row>
+    <row r="40" spans="2:7" ht="25.5">
+      <c r="B40" s="110"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="111" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="59"/>
+      <c r="G40" s="67"/>
+    </row>
+    <row r="41" spans="2:7" ht="39" thickBot="1">
+      <c r="B41" s="112"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="60"/>
+      <c r="G41" s="68"/>
+    </row>
+    <row r="42" spans="2:7" ht="38.25">
+      <c r="B42" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="103" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="G42" s="85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="38.25">
+      <c r="B43" s="114"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="38.25">
+      <c r="B44" s="114"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="67"/>
+    </row>
+    <row r="45" spans="2:7" ht="38.25">
+      <c r="B45" s="114"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" s="59"/>
+      <c r="G45" s="67"/>
+    </row>
+    <row r="46" spans="2:7" ht="39" thickBot="1">
+      <c r="B46" s="116"/>
+      <c r="C46" s="117"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="60"/>
+      <c r="G46" s="68"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="E47" s="13"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="E48" s="13"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="5:7">
+      <c r="E49" s="13"/>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="5:7">
+      <c r="E50" s="13"/>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="5:7">
+      <c r="E51" s="13"/>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="5:7">
+      <c r="E52" s="13"/>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="5:7">
+      <c r="E53" s="13"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="5:7">
+      <c r="E54" s="13"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="5:7">
+      <c r="E55" s="13"/>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="5:7">
+      <c r="E56" s="13"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="5:7">
+      <c r="E57" s="13"/>
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="5:7">
+      <c r="E58" s="13"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59" spans="5:7">
+      <c r="E59" s="13"/>
+      <c r="G59" s="13"/>
+    </row>
+    <row r="60" spans="5:7">
+      <c r="E60" s="13"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="5:7">
+      <c r="E61" s="13"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="5:7">
+      <c r="E62" s="13"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="5:7">
+      <c r="E63" s="13"/>
+      <c r="G63" s="13"/>
+    </row>
+    <row r="64" spans="5:7">
+      <c r="E64" s="13"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="5:7">
+      <c r="E65" s="13"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="5:7">
+      <c r="G66" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="36">
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="D19:D22"/>
@@ -1226,19 +2245,14 @@
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1" display="https://refactoring.guru/ru/design-patterns/factory-method"/>
     <hyperlink ref="E18" r:id="rId2" display="https://refactoring.guru/ru/design-patterns/composite"/>
+    <hyperlink ref="G35" r:id="rId3" display="https://refactoring.guru/ru/antipatterns/god-object"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added Behavioral patterns group
</commit_message>
<xml_diff>
--- a/Patterns.xlsx
+++ b/Patterns.xlsx
@@ -915,84 +915,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,150 +943,228 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1471,7 +1471,7 @@
   <dimension ref="A2:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C28"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1511,13 +1511,13 @@
       <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="95" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1532,9 +1532,9 @@
     </row>
     <row r="4" spans="1:7" ht="25.5">
       <c r="A4" s="32"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="51"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1547,9 +1547,9 @@
     </row>
     <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="32"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
         <v>5</v>
@@ -1560,9 +1560,9 @@
     </row>
     <row r="6" spans="1:7" ht="26.25" thickBot="1">
       <c r="A6" s="32"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="52"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
       <c r="G6" s="30" t="s">
@@ -1573,13 +1573,13 @@
       <c r="A7" s="32">
         <v>2</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="103" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1594,9 +1594,9 @@
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1">
       <c r="A8" s="32"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="57"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1607,9 +1607,9 @@
     </row>
     <row r="9" spans="1:7" ht="38.25" customHeight="1">
       <c r="A9" s="32"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="57"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="104"/>
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1620,9 +1620,9 @@
     </row>
     <row r="10" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
       <c r="A10" s="32"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="105"/>
       <c r="E10" s="9"/>
       <c r="F10" s="11" t="s">
         <v>28</v>
@@ -1633,13 +1633,13 @@
       <c r="A11" s="32">
         <v>3</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="110" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1654,9 +1654,9 @@
     </row>
     <row r="12" spans="1:7" ht="38.25">
       <c r="A12" s="32"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="43"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="111"/>
       <c r="E12" s="17" t="s">
         <v>22</v>
       </c>
@@ -1669,9 +1669,9 @@
     </row>
     <row r="13" spans="1:7" ht="25.5">
       <c r="A13" s="32"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="43"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="4"/>
       <c r="F13" s="24" t="s">
         <v>18</v>
@@ -1680,9 +1680,9 @@
     </row>
     <row r="14" spans="1:7" ht="25.5">
       <c r="A14" s="32"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="43"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="4"/>
       <c r="F14" s="24" t="s">
         <v>19</v>
@@ -1691,9 +1691,9 @@
     </row>
     <row r="15" spans="1:7" ht="26.25" thickBot="1">
       <c r="A15" s="32"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="112"/>
       <c r="E15" s="9"/>
       <c r="F15" s="25" t="s">
         <v>28</v>
@@ -1704,13 +1704,13 @@
       <c r="A16" s="32">
         <v>4</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="115" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1725,9 +1725,9 @@
     </row>
     <row r="17" spans="1:7" ht="38.25">
       <c r="A17" s="32"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="48"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="116"/>
       <c r="E17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1740,9 +1740,9 @@
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1">
       <c r="A18" s="32"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="49"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="117"/>
       <c r="E18" s="18" t="s">
         <v>35</v>
       </c>
@@ -1755,13 +1755,13 @@
       <c r="A19" s="32">
         <v>5</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="103" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1776,9 +1776,9 @@
     </row>
     <row r="20" spans="1:7" ht="51">
       <c r="A20" s="32"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="40"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="5" t="s">
         <v>46</v>
       </c>
@@ -1789,9 +1789,9 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="32"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="40"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="108"/>
       <c r="E21" s="5"/>
       <c r="F21" s="21" t="s">
         <v>49</v>
@@ -1800,9 +1800,9 @@
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1">
       <c r="A22" s="32"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="109"/>
       <c r="E22" s="10"/>
       <c r="F22" s="22" t="s">
         <v>50</v>
@@ -1811,322 +1811,322 @@
     </row>
     <row r="23" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="24" spans="1:7" ht="38.25">
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="84" t="s">
+      <c r="E24" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="84" t="s">
+      <c r="F24" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="85" t="s">
+      <c r="G24" s="44" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="51.75" thickBot="1">
       <c r="B25" s="86"/>
       <c r="C25" s="87"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="62" t="s">
+      <c r="D25" s="88"/>
+      <c r="E25" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="62" t="s">
+      <c r="F25" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="68" t="s">
+      <c r="G25" s="42" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="51">
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="83" t="s">
+      <c r="C26" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="88" t="s">
+      <c r="E26" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="89" t="s">
+      <c r="F26" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="38"/>
     </row>
     <row r="27" spans="1:7" ht="25.5">
-      <c r="B27" s="90"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="91" t="s">
+      <c r="B27" s="89"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="92" t="s">
+      <c r="F27" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="65"/>
+      <c r="G27" s="39"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" thickBot="1">
-      <c r="B28" s="93"/>
-      <c r="C28" s="79"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="72"/>
-      <c r="E28" s="94" t="s">
+      <c r="E28" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="63"/>
-      <c r="G28" s="66"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" ht="25.5">
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="69" t="s">
+      <c r="D29" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="95" t="s">
+      <c r="E29" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="F29" s="95" t="s">
+      <c r="F29" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="96" t="s">
+      <c r="G29" s="51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="26.25" thickBot="1">
-      <c r="B30" s="97"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="99" t="s">
+      <c r="B30" s="71"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="99" t="s">
+      <c r="F30" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="66"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:7" ht="25.5">
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="83" t="s">
+      <c r="C31" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="74" t="s">
+      <c r="D31" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="84" t="s">
+      <c r="E31" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="84" t="s">
+      <c r="F31" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="85" t="s">
+      <c r="G31" s="44" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="25.5">
-      <c r="B32" s="100"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="61" t="s">
+      <c r="B32" s="84"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="61" t="s">
+      <c r="F32" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="G32" s="67" t="s">
+      <c r="G32" s="41" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="25.5">
-      <c r="B33" s="100"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61" t="s">
+      <c r="B33" s="84"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="67"/>
+      <c r="G33" s="41"/>
     </row>
     <row r="34" spans="2:7" ht="26.25" thickBot="1">
-      <c r="B34" s="101"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62" t="s">
+      <c r="B34" s="85"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G34" s="68"/>
+      <c r="G34" s="42"/>
     </row>
     <row r="35" spans="2:7" ht="25.5">
-      <c r="B35" s="82" t="s">
+      <c r="B35" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="102" t="s">
+      <c r="C35" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="69" t="s">
+      <c r="D35" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="103" t="s">
+      <c r="E35" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="84" t="s">
+      <c r="F35" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="104" t="s">
+      <c r="G35" s="54" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="26.25" thickBot="1">
-      <c r="B36" s="97"/>
-      <c r="C36" s="105"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="72"/>
-      <c r="E36" s="106" t="s">
+      <c r="E36" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="60"/>
-      <c r="G36" s="68"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="42"/>
     </row>
     <row r="37" spans="2:7" ht="25.5">
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C37" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="77" t="s">
+      <c r="D37" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="108" t="s">
+      <c r="E37" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="F37" s="109" t="s">
+      <c r="F37" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="G37" s="85" t="s">
+      <c r="G37" s="44" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="25.5">
-      <c r="B38" s="110"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="111" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="67" t="s">
+      <c r="F38" s="33"/>
+      <c r="G38" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="110"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="111" t="s">
+      <c r="B39" s="77"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="F39" s="59"/>
-      <c r="G39" s="67"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="41"/>
     </row>
     <row r="40" spans="2:7" ht="25.5">
-      <c r="B40" s="110"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="111" t="s">
+      <c r="B40" s="77"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="59"/>
-      <c r="G40" s="67"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="41"/>
     </row>
     <row r="41" spans="2:7" ht="39" thickBot="1">
-      <c r="B41" s="112"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="106" t="s">
+      <c r="B41" s="78"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F41" s="60"/>
-      <c r="G41" s="68"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="42"/>
     </row>
     <row r="42" spans="2:7" ht="38.25">
-      <c r="B42" s="107" t="s">
+      <c r="B42" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="113" t="s">
+      <c r="C42" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="69" t="s">
+      <c r="D42" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="103" t="s">
+      <c r="E42" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="84" t="s">
+      <c r="F42" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G42" s="85" t="s">
+      <c r="G42" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="38.25">
-      <c r="B43" s="114"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="111" t="s">
+      <c r="B43" s="60"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="61" t="s">
+      <c r="F43" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G43" s="67" t="s">
+      <c r="G43" s="41" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="38.25">
-      <c r="B44" s="114"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="61" t="s">
+      <c r="B44" s="60"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="61" t="s">
+      <c r="F44" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="G44" s="67"/>
+      <c r="G44" s="41"/>
     </row>
     <row r="45" spans="2:7" ht="38.25">
-      <c r="B45" s="114"/>
-      <c r="C45" s="115"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="61" t="s">
+      <c r="B45" s="60"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="59"/>
-      <c r="G45" s="67"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="41"/>
     </row>
     <row r="46" spans="2:7" ht="39" thickBot="1">
-      <c r="B46" s="116"/>
-      <c r="C46" s="117"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="62" t="s">
+      <c r="B46" s="61"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="60"/>
-      <c r="G46" s="68"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="42"/>
     </row>
     <row r="47" spans="2:7">
       <c r="E47" s="13"/>
@@ -2209,6 +2209,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B31:B34"/>
     <mergeCell ref="B42:B46"/>
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="D42:D46"/>
@@ -2218,33 +2245,6 @@
     <mergeCell ref="D37:D41"/>
     <mergeCell ref="C37:C41"/>
     <mergeCell ref="B37:B41"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1" display="https://refactoring.guru/ru/design-patterns/factory-method"/>

</xml_diff>